<commit_message>
Objectstructuur netter zodat ook runtime de wedstrijdinstellingen aangepast kunnen worden
</commit_message>
<xml_diff>
--- a/Spelers/NT WC18 Skills.xlsx
+++ b/Spelers/NT WC18 Skills.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="405" windowWidth="18915" windowHeight="11535" tabRatio="781"/>
+    <workbookView xWindow="240" yWindow="405" windowWidth="18915" windowHeight="11535" tabRatio="781" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PB vrijdag" sheetId="14" r:id="rId1"/>
-    <sheet name="PB donderdag" sheetId="13" r:id="rId2"/>
+    <sheet name="PB toekomst" sheetId="13" r:id="rId2"/>
     <sheet name="UAE - 1203" sheetId="1" r:id="rId3"/>
     <sheet name="DomRep - 0203" sheetId="2" r:id="rId4"/>
     <sheet name="MAL-1203" sheetId="3" r:id="rId5"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="466">
   <si>
     <t>Naam</t>
   </si>
@@ -1413,6 +1413,18 @@
   </si>
   <si>
     <t>Constantijn van der Sterren</t>
+  </si>
+  <si>
+    <t>WB</t>
+  </si>
+  <si>
+    <t>WTM</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>tDFW</t>
   </si>
 </sst>
 </file>
@@ -1641,7 +1653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1772,6 +1784,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2077,8 +2092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11696,10 +11711,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11719,9 +11734,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
-        <v>411</v>
-      </c>
+      <c r="A1" s="62"/>
       <c r="B1" s="63" t="s">
         <v>0</v>
       </c>
@@ -11763,9 +11776,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
-        <v>12</v>
-      </c>
+      <c r="A2" s="62"/>
       <c r="B2" t="s">
         <v>433</v>
       </c>
@@ -11773,10 +11784,10 @@
         <v>13</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -11785,7 +11796,7 @@
         <v>6</v>
       </c>
       <c r="H2">
-        <v>15.13</v>
+        <v>19.3</v>
       </c>
       <c r="I2">
         <v>5</v>
@@ -11800,36 +11811,34 @@
         <v>19</v>
       </c>
       <c r="M2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N2" s="62">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
-        <v>12</v>
-      </c>
+      <c r="A3" s="62"/>
       <c r="B3" t="s">
         <v>434</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D3">
         <v>6</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3">
-        <v>5.3</v>
+        <v>11</v>
       </c>
       <c r="I3">
         <v>4</v>
@@ -11844,10 +11853,10 @@
         <v>1</v>
       </c>
       <c r="M3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N3" s="62">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -11855,12 +11864,14 @@
       <c r="B4" t="s">
         <v>435</v>
       </c>
-      <c r="C4" s="64"/>
+      <c r="C4" s="64" t="s">
+        <v>39</v>
+      </c>
       <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
         <v>8</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -11869,7 +11880,7 @@
         <v>15</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -11884,27 +11895,25 @@
         <v>4</v>
       </c>
       <c r="M4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N4" s="62">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
-        <v>12</v>
-      </c>
+      <c r="A5" s="62"/>
       <c r="B5" t="s">
         <v>436</v>
       </c>
       <c r="C5" s="65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>6</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -11913,7 +11922,7 @@
         <v>10.15</v>
       </c>
       <c r="H5">
-        <v>12.31</v>
+        <v>18.5</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -11928,16 +11937,14 @@
         <v>3</v>
       </c>
       <c r="M5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N5" s="62">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
-        <v>12</v>
-      </c>
+      <c r="A6" s="62"/>
       <c r="B6" t="s">
         <v>437</v>
       </c>
@@ -11948,7 +11955,7 @@
         <v>6</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -11957,7 +11964,7 @@
         <v>10</v>
       </c>
       <c r="H6">
-        <v>13.3</v>
+        <v>18.7</v>
       </c>
       <c r="I6">
         <v>3</v>
@@ -11972,39 +11979,37 @@
         <v>1</v>
       </c>
       <c r="M6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N6" s="62">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
-        <v>12</v>
-      </c>
+      <c r="A7" s="62"/>
       <c r="B7" t="s">
-        <v>438</v>
+        <v>462</v>
       </c>
       <c r="C7" s="64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>15.32</v>
+        <v>15</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="J7">
         <v>8</v>
@@ -12016,16 +12021,14 @@
         <v>1</v>
       </c>
       <c r="M7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N7" s="62">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="62" t="s">
-        <v>12</v>
-      </c>
+      <c r="A8" s="62"/>
       <c r="B8" t="s">
         <v>439</v>
       </c>
@@ -12036,13 +12039,13 @@
         <v>6</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <v>15</v>
       </c>
       <c r="G8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -12060,27 +12063,25 @@
         <v>2</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="N8" s="62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="62"/>
+      <c r="B9" t="s">
+        <v>463</v>
+      </c>
+      <c r="C9" s="64" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>440</v>
-      </c>
-      <c r="C9" s="64" t="s">
-        <v>19</v>
-      </c>
       <c r="D9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -12089,7 +12090,7 @@
         <v>12</v>
       </c>
       <c r="H9">
-        <v>9.2200000000000006</v>
+        <v>17</v>
       </c>
       <c r="I9">
         <v>5</v>
@@ -12104,71 +12105,66 @@
         <v>1</v>
       </c>
       <c r="M9">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="N9" s="62">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="s">
-        <v>12</v>
-      </c>
       <c r="B10" t="s">
-        <v>441</v>
-      </c>
-      <c r="C10" s="64" t="s">
-        <v>14</v>
+        <v>459</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
         <v>3</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>7</v>
-      </c>
-      <c r="H10">
-        <v>8</v>
-      </c>
       <c r="I10">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J10">
         <v>7</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N10" s="62">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="62"/>
+      <c r="B11" t="s">
+        <v>464</v>
+      </c>
+      <c r="C11" s="64" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>442</v>
-      </c>
-      <c r="C11" s="64" t="s">
-        <v>19</v>
-      </c>
       <c r="D11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -12180,13 +12176,13 @@
         <v>3</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K11">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L11">
         <v>2</v>
@@ -12195,15 +12191,13 @@
         <v>10</v>
       </c>
       <c r="N11" s="62">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="s">
-        <v>12</v>
-      </c>
+      <c r="A12" s="62"/>
       <c r="B12" t="s">
-        <v>443</v>
+        <v>464</v>
       </c>
       <c r="C12" s="64" t="s">
         <v>14</v>
@@ -12212,7 +12206,7 @@
         <v>6</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -12224,35 +12218,37 @@
         <v>5</v>
       </c>
       <c r="I12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J12">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K12">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L12">
         <v>2</v>
       </c>
       <c r="M12">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N12" s="62">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="62"/>
       <c r="B13" t="s">
-        <v>444</v>
-      </c>
-      <c r="C13" s="64"/>
+        <v>464</v>
+      </c>
+      <c r="C13" s="64" t="s">
+        <v>16</v>
+      </c>
       <c r="D13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -12264,39 +12260,37 @@
         <v>2</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J13">
         <v>9</v>
       </c>
       <c r="K13">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L13">
         <v>7</v>
       </c>
       <c r="M13">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="N13" s="62">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="s">
-        <v>12</v>
-      </c>
+      <c r="A14" s="62"/>
       <c r="B14" t="s">
-        <v>445</v>
+        <v>465</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D14">
         <v>6</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -12305,700 +12299,96 @@
         <v>3</v>
       </c>
       <c r="H14">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
         <v>14</v>
       </c>
-      <c r="J14">
-        <v>5</v>
-      </c>
       <c r="K14">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="L14">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="N14" s="62">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>447</v>
-      </c>
-      <c r="C15" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15">
-        <v>8</v>
-      </c>
-      <c r="E15">
-        <v>4</v>
-      </c>
-      <c r="F15">
-        <v>6</v>
-      </c>
-      <c r="G15">
-        <v>3</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>5</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15" s="62">
-        <v>15</v>
-      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>448</v>
-      </c>
-      <c r="C16" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16">
-        <v>6</v>
-      </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-      <c r="I16">
-        <v>13</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>5</v>
-      </c>
-      <c r="M16">
-        <v>11</v>
-      </c>
-      <c r="N16" s="62">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>449</v>
-      </c>
-      <c r="C17" s="64" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>3</v>
-      </c>
-      <c r="H17">
-        <v>11</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>11</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17">
-        <v>13</v>
-      </c>
-      <c r="N17" s="62">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>450</v>
-      </c>
-      <c r="C18" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18">
-        <v>4</v>
-      </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>5</v>
-      </c>
-      <c r="H18">
-        <v>8</v>
-      </c>
-      <c r="I18">
-        <v>2</v>
-      </c>
-      <c r="J18">
-        <v>4</v>
-      </c>
-      <c r="K18">
-        <v>2</v>
-      </c>
-      <c r="L18">
-        <v>2</v>
-      </c>
-      <c r="M18">
-        <v>2</v>
-      </c>
-      <c r="N18" s="62">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" t="s">
-        <v>451</v>
-      </c>
-      <c r="C19" s="64" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19">
-        <v>6</v>
-      </c>
-      <c r="E19">
-        <v>4</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>5</v>
-      </c>
-      <c r="H19">
-        <v>6</v>
-      </c>
-      <c r="I19">
-        <v>4</v>
-      </c>
-      <c r="J19">
-        <v>4</v>
-      </c>
-      <c r="K19">
-        <v>4</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <v>2</v>
-      </c>
-      <c r="N19" s="62">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
-      <c r="B20" t="s">
-        <v>452</v>
-      </c>
-      <c r="C20" s="64"/>
-      <c r="D20">
-        <v>5</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>5</v>
-      </c>
-      <c r="H20">
-        <v>6</v>
-      </c>
-      <c r="I20">
-        <v>5</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <v>4</v>
-      </c>
-      <c r="L20">
-        <v>2</v>
-      </c>
-      <c r="M20">
-        <v>2</v>
-      </c>
-      <c r="N20" s="62">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" t="s">
-        <v>453</v>
-      </c>
-      <c r="C21" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21">
-        <v>5</v>
-      </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>6</v>
-      </c>
-      <c r="H21">
-        <v>5</v>
-      </c>
-      <c r="I21">
-        <v>4</v>
-      </c>
-      <c r="J21">
-        <v>3</v>
-      </c>
-      <c r="K21">
-        <v>4</v>
-      </c>
-      <c r="L21">
-        <v>3</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21" s="62">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" t="s">
-        <v>454</v>
-      </c>
-      <c r="C22" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22">
-        <v>7</v>
-      </c>
-      <c r="E22">
-        <v>3</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>5</v>
-      </c>
-      <c r="H22">
-        <v>4</v>
-      </c>
-      <c r="I22">
-        <v>2</v>
-      </c>
-      <c r="J22">
-        <v>5</v>
-      </c>
-      <c r="K22">
-        <v>3</v>
-      </c>
-      <c r="L22">
-        <v>4</v>
-      </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22" s="62">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
-      <c r="B23" t="s">
-        <v>455</v>
-      </c>
-      <c r="C23" s="64"/>
-      <c r="D23">
-        <v>6</v>
-      </c>
-      <c r="E23">
-        <v>3</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>4</v>
-      </c>
-      <c r="H23">
-        <v>4</v>
-      </c>
-      <c r="I23">
-        <v>6</v>
-      </c>
-      <c r="J23">
-        <v>4</v>
-      </c>
-      <c r="K23">
-        <v>4</v>
-      </c>
-      <c r="L23">
-        <v>5</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23" s="62">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
-        <v>456</v>
-      </c>
-      <c r="C24" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24">
-        <v>4</v>
-      </c>
-      <c r="E24">
-        <v>3</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>7</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>7</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>2</v>
-      </c>
-      <c r="M24">
-        <v>7</v>
-      </c>
-      <c r="N24" s="62">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" t="s">
-        <v>457</v>
-      </c>
-      <c r="C25" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25">
-        <v>6</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>3</v>
-      </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
-      <c r="I25">
-        <v>4</v>
-      </c>
-      <c r="J25">
-        <v>5</v>
-      </c>
-      <c r="K25">
-        <v>2</v>
-      </c>
-      <c r="L25">
-        <v>7</v>
-      </c>
-      <c r="M25">
-        <v>4</v>
-      </c>
-      <c r="N25" s="62">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
-      <c r="B26" t="s">
-        <v>458</v>
-      </c>
-      <c r="C26" s="64"/>
-      <c r="D26">
-        <v>5</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>5</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
-        <v>10</v>
-      </c>
-      <c r="N26" s="62">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" t="s">
-        <v>459</v>
-      </c>
-      <c r="C27" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27">
-        <v>7</v>
-      </c>
-      <c r="E27">
-        <v>7</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>4</v>
-      </c>
-      <c r="H27">
-        <v>3</v>
-      </c>
-      <c r="I27">
-        <v>17</v>
-      </c>
-      <c r="J27">
-        <v>7</v>
-      </c>
-      <c r="K27">
-        <v>3</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
-      <c r="M27">
-        <v>3</v>
-      </c>
-      <c r="N27" s="62">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" t="s">
-        <v>461</v>
-      </c>
-      <c r="C28" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28">
-        <v>6</v>
-      </c>
-      <c r="E28">
-        <v>4</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>4</v>
-      </c>
-      <c r="H28">
-        <v>5</v>
-      </c>
-      <c r="I28">
-        <v>3</v>
-      </c>
-      <c r="J28">
-        <v>7</v>
-      </c>
-      <c r="K28">
-        <v>4</v>
-      </c>
-      <c r="L28">
-        <v>3</v>
-      </c>
-      <c r="M28">
-        <v>1</v>
-      </c>
-      <c r="N28" s="62">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Creatief met getallen. Mid+Def iets hoger. Een magic number om de aanval gelijk aan HO te trekken (lager)
</commit_message>
<xml_diff>
--- a/Spelers/NT WC18 Skills.xlsx
+++ b/Spelers/NT WC18 Skills.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="405" windowWidth="18915" windowHeight="11535" tabRatio="781" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="405" windowWidth="18915" windowHeight="11535" tabRatio="781"/>
   </bookViews>
   <sheets>
     <sheet name="PB vrijdag" sheetId="14" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="465">
   <si>
     <t>Naam</t>
   </si>
@@ -1410,9 +1410,6 @@
   </si>
   <si>
     <t>LOY</t>
-  </si>
-  <si>
-    <t>Constantijn van der Sterren</t>
   </si>
   <si>
     <t>WB</t>
@@ -2092,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:N27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,7 +2164,7 @@
         <v>13</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -2179,7 +2176,7 @@
         <v>6</v>
       </c>
       <c r="H2">
-        <v>15.13</v>
+        <v>15.64</v>
       </c>
       <c r="I2">
         <v>5</v>
@@ -2197,7 +2194,7 @@
         <v>7</v>
       </c>
       <c r="N2" s="62">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -2307,7 +2304,7 @@
         <v>10.15</v>
       </c>
       <c r="H5">
-        <v>12.47</v>
+        <v>13.14</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -2351,7 +2348,7 @@
         <v>10</v>
       </c>
       <c r="H6">
-        <v>13.44</v>
+        <v>14.14</v>
       </c>
       <c r="I6">
         <v>3</v>
@@ -3198,130 +3195,132 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="62"/>
-      <c r="B26" t="s">
-        <v>458</v>
-      </c>
-      <c r="C26" s="64"/>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="64" t="s">
+        <v>14</v>
+      </c>
       <c r="D26">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H26">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M26">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="N26" s="62">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B27" t="s">
-        <v>459</v>
+      <c r="B27">
+        <v>2</v>
       </c>
       <c r="C27" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E27">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H27">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="I27">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="J27">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K27">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N27" s="62">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B28" t="s">
-        <v>461</v>
+      <c r="B28">
+        <v>3</v>
       </c>
       <c r="C28" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E28">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H28">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I28">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J28">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K28">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="L28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N28" s="62">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -11713,7 +11712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -11988,7 +11987,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="62"/>
       <c r="B7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C7" s="64" t="s">
         <v>14</v>
@@ -12072,7 +12071,7 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="62"/>
       <c r="B9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C9" s="64" t="s">
         <v>14</v>
@@ -12155,7 +12154,7 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="62"/>
       <c r="B11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C11" s="64" t="s">
         <v>16</v>
@@ -12197,7 +12196,7 @@
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="62"/>
       <c r="B12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C12" s="64" t="s">
         <v>14</v>
@@ -12239,7 +12238,7 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="62"/>
       <c r="B13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C13" s="64" t="s">
         <v>16</v>
@@ -12281,7 +12280,7 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="62"/>
       <c r="B14" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C14" s="64" t="s">
         <v>19</v>

</xml_diff>